<commit_message>
Edit studi kasus, form dan visualisasi data kasus
</commit_message>
<xml_diff>
--- a/studi-kasus/studi-kasus.xlsx
+++ b/studi-kasus/studi-kasus.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mughi\Downloads\travlendar-docs-mockups\studi-kasus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mughi\College\Semester 3\Project 3\travlendar-docs-mockups\studi-kasus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Studi Kasus" sheetId="4" r:id="rId1"/>
-    <sheet name="From" sheetId="5" r:id="rId2"/>
-    <sheet name="Example" sheetId="1" r:id="rId3"/>
+    <sheet name="Example" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="115">
   <si>
     <t>Nama Kegiatan</t>
   </si>
@@ -378,27 +377,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>Form</t>
-  </si>
-  <si>
-    <t>User Input</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>Add Activity</t>
-  </si>
-  <si>
-    <t>Add Location</t>
-  </si>
-  <si>
-    <t>Create Schedule</t>
-  </si>
-  <si>
-    <t>Date Schedule</t>
-  </si>
-  <si>
     <t>Activity's Title</t>
   </si>
   <si>
@@ -408,21 +386,6 @@
     <t>Time Activity Ended</t>
   </si>
   <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>To (Destination)</t>
-  </si>
-  <si>
-    <t>Address To (Destination)</t>
-  </si>
-  <si>
-    <t>Distance (From - To)</t>
-  </si>
-  <si>
     <t>Time Zone</t>
   </si>
   <si>
@@ -432,9 +395,6 @@
     <t>Transportation Mode</t>
   </si>
   <si>
-    <t>Estimation Time</t>
-  </si>
-  <si>
     <t>Dalam mengatur jadwal biasanya Bu Sitti akan berkomunikasi dengan orang yang bersangkutan terkait konfirmasi akan dilaksanakan atau tidaknya acara.</t>
   </si>
   <si>
@@ -474,34 +434,7 @@
     <t>Program travlendar ini akan memberikan rekomendasi kendaraan yang akan digunakan oleh user untuk bepergian termasuk kendaraan umum untuk mengefisienkan waktu perjalanan</t>
   </si>
   <si>
-    <t>From (Starting Point)</t>
-  </si>
-  <si>
-    <t>Address From (Starting Point)</t>
-  </si>
-  <si>
     <t>Program travlendar ini juga akan merekomendasikan waktu keberangkatan user agar dapat datang pada suatu kegiatan dengan tepat waktu</t>
-  </si>
-  <si>
-    <t>Data Transaksi</t>
-  </si>
-  <si>
-    <t>Data Master</t>
-  </si>
-  <si>
-    <t>Di inputkan oleh user</t>
-  </si>
-  <si>
-    <t>Di dapatkan dari perhitungan system (Time Activity Started - Estimation Time)</t>
-  </si>
-  <si>
-    <t>Di inputkan oleh admin/pengembang untuk mendapatkan data Estimation Time</t>
-  </si>
-  <si>
-    <t>Di dapatkan dari perhitungan system (Jarak - Transportation Mode [Velocity])</t>
-  </si>
-  <si>
-    <t>Starting Point</t>
   </si>
 </sst>
 </file>
@@ -513,7 +446,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,24 +477,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -589,12 +506,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -771,7 +682,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,7 +736,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,30 +747,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,15 +1049,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.44140625" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.77734375" style="26" bestFit="1" customWidth="1"/>
@@ -1188,56 +1089,56 @@
       <c r="A2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
@@ -1261,64 +1162,64 @@
       <c r="A7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
+      <c r="B7" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
@@ -1329,51 +1230,51 @@
       <c r="A12" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
+        <v>98</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
@@ -1400,13 +1301,13 @@
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="51" t="s">
+      <c r="J14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
@@ -1433,11 +1334,11 @@
       <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
@@ -1464,11 +1365,11 @@
       <c r="I16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
@@ -1495,11 +1396,11 @@
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
@@ -1526,11 +1427,11 @@
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
@@ -1557,11 +1458,11 @@
       <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
@@ -1588,14 +1489,14 @@
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="65" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1606,64 +1507,64 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
     </row>
     <row r="26" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -1717,28 +1618,28 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="41">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F29" s="42" t="s">
+      <c r="F29" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="42">
+      <c r="G29" s="41">
         <v>0.5</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="39">
         <v>1</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="39" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1832,51 +1733,51 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="38" t="s">
         <v>81</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J36" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="K36" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J36" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="K36" s="44" t="s">
-        <v>115</v>
-      </c>
       <c r="L36" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37" s="15">
         <v>1</v>
       </c>
-      <c r="C37" s="48">
+      <c r="C37" s="47">
         <v>42997</v>
       </c>
       <c r="D37" s="17" t="s">
@@ -1914,7 +1815,7 @@
       <c r="B38" s="15">
         <v>2</v>
       </c>
-      <c r="C38" s="48"/>
+      <c r="C38" s="47"/>
       <c r="D38" s="17" t="s">
         <v>72</v>
       </c>
@@ -1950,7 +1851,7 @@
       <c r="B39" s="15">
         <v>3</v>
       </c>
-      <c r="C39" s="48"/>
+      <c r="C39" s="47"/>
       <c r="D39" s="17" t="s">
         <v>74</v>
       </c>
@@ -1986,7 +1887,7 @@
       <c r="B40" s="15">
         <v>4</v>
       </c>
-      <c r="C40" s="48"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="25" t="s">
         <v>58</v>
       </c>
@@ -2022,7 +1923,7 @@
       <c r="B41" s="15">
         <v>5</v>
       </c>
-      <c r="C41" s="48"/>
+      <c r="C41" s="47"/>
       <c r="D41" s="17" t="s">
         <v>57</v>
       </c>
@@ -2058,11 +1959,11 @@
       <c r="B42" s="15">
         <v>6</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="45" t="s">
+      <c r="C42" s="47"/>
+      <c r="D42" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="44" t="s">
         <v>68</v>
       </c>
       <c r="F42" s="17" t="s">
@@ -2094,11 +1995,11 @@
       <c r="B43" s="15">
         <v>7</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="45" t="s">
+      <c r="C43" s="47"/>
+      <c r="D43" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="44" t="s">
         <v>66</v>
       </c>
       <c r="F43" s="17" t="s">
@@ -2125,6 +2026,129 @@
       <c r="M43" s="15" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="61"/>
+      <c r="B46" s="56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="63"/>
+      <c r="B48" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="56"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="63"/>
+      <c r="B49" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="56"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="63"/>
+      <c r="B51" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="56"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="63"/>
+      <c r="B52" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="56"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="61"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="58"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="58"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" s="58"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="59"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2143,350 +2167,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="58" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.33203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="58"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="61" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="60"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="60"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="60"/>
-    </row>
-    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="61"/>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="60"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="64" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-    </row>
-    <row r="18" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="66" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="66" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" s="68"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="68"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="D26" s="68"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="69" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="69" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="64" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="66" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="58" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D33" s="58" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" s="58" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="58" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="58" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="66" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="71" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D40" s="58" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="70" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="58" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="70" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
@@ -2787,25 +2467,25 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="42">
         <v>0.29166666666666669</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="42">
         <v>0.375</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="39">
         <v>2</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H21" s="39" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2898,7 +2578,7 @@
       <c r="H27" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="54" t="s">
+      <c r="I27" s="53" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2924,31 +2604,31 @@
       <c r="H28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="55"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="42">
         <v>0.29166666666666669</v>
       </c>
-      <c r="F29" s="43">
+      <c r="F29" s="42">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="39">
         <v>4</v>
       </c>
-      <c r="H29" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="55"/>
+      <c r="H29" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="54"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
@@ -2972,7 +2652,7 @@
       <c r="H30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="56"/>
+      <c r="I30" s="55"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -2992,12 +2672,12 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>